<commit_message>
Count dels/dups per ethnicity
</commit_message>
<xml_diff>
--- a/docs/QA.xlsx
+++ b/docs/QA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tristan\Mython\Myriad\deldup\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F1FA7E-8623-4D97-B0FC-ABBD5BEA6804}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC160F0-3D71-4843-8B13-52AA57A851D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15855" yWindow="45" windowWidth="12480" windowHeight="15075" xr2:uid="{899D5349-A592-411E-BDDE-F0AD4F05CE2C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="11">
   <si>
     <t>label</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>bisect</t>
+  </si>
+  <si>
+    <t>std*2</t>
+  </si>
+  <si>
+    <t>skewed</t>
   </si>
 </sst>
 </file>
@@ -108,7 +114,775 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="228">
+  <dxfs count="324">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -2243,15 +3017,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63000581-C07F-4440-90FE-8419FD7252C1}">
-  <dimension ref="A1:N51"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="N43" sqref="N43"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2288,8 +3062,14 @@
       <c r="N1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2323,8 +3103,14 @@
       <c r="N2" t="s">
         <v>4</v>
       </c>
+      <c r="O2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>1</v>
@@ -2361,8 +3147,14 @@
       <c r="N3" t="s">
         <v>4</v>
       </c>
+      <c r="O3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A53" si="0">A3+1</f>
         <v>2</v>
@@ -2399,8 +3191,14 @@
       <c r="N4" t="s">
         <v>4</v>
       </c>
+      <c r="O4" t="s">
+        <v>4</v>
+      </c>
+      <c r="P4" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -2437,8 +3235,14 @@
       <c r="N5" t="s">
         <v>4</v>
       </c>
+      <c r="O5" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2475,8 +3279,14 @@
       <c r="N6" t="s">
         <v>4</v>
       </c>
+      <c r="O6" t="s">
+        <v>4</v>
+      </c>
+      <c r="P6" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2513,8 +3323,14 @@
       <c r="N7" t="s">
         <v>4</v>
       </c>
+      <c r="O7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P7" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2551,8 +3367,14 @@
       <c r="N8" t="s">
         <v>4</v>
       </c>
+      <c r="O8" t="s">
+        <v>4</v>
+      </c>
+      <c r="P8" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2589,8 +3411,14 @@
       <c r="N9" t="s">
         <v>4</v>
       </c>
+      <c r="O9" t="s">
+        <v>4</v>
+      </c>
+      <c r="P9" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2627,8 +3455,14 @@
       <c r="N10" t="s">
         <v>4</v>
       </c>
+      <c r="O10" t="s">
+        <v>4</v>
+      </c>
+      <c r="P10" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2665,8 +3499,14 @@
       <c r="N11" t="s">
         <v>4</v>
       </c>
+      <c r="O11" t="s">
+        <v>4</v>
+      </c>
+      <c r="P11" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2706,8 +3546,14 @@
       <c r="N12" t="s">
         <v>4</v>
       </c>
+      <c r="O12" t="s">
+        <v>4</v>
+      </c>
+      <c r="P12" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2747,8 +3593,14 @@
       <c r="N13" t="s">
         <v>5</v>
       </c>
+      <c r="O13" t="s">
+        <v>4</v>
+      </c>
+      <c r="P13" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2788,8 +3640,14 @@
       <c r="N14" t="s">
         <v>4</v>
       </c>
+      <c r="O14" t="s">
+        <v>4</v>
+      </c>
+      <c r="P14" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2824,13 +3682,19 @@
         <v>3</v>
       </c>
       <c r="M15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N15" t="s">
         <v>5</v>
       </c>
+      <c r="O15" t="s">
+        <v>5</v>
+      </c>
+      <c r="P15" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2870,8 +3734,14 @@
       <c r="N16" t="s">
         <v>5</v>
       </c>
+      <c r="O16" t="s">
+        <v>5</v>
+      </c>
+      <c r="P16" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2911,8 +3781,14 @@
       <c r="N17" t="s">
         <v>4</v>
       </c>
+      <c r="O17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P17" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2952,8 +3828,14 @@
       <c r="N18" t="s">
         <v>4</v>
       </c>
+      <c r="O18" t="s">
+        <v>4</v>
+      </c>
+      <c r="P18" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2993,8 +3875,14 @@
       <c r="N19" t="s">
         <v>4</v>
       </c>
+      <c r="O19" t="s">
+        <v>4</v>
+      </c>
+      <c r="P19" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3034,8 +3922,14 @@
       <c r="N20" t="s">
         <v>5</v>
       </c>
+      <c r="O20" t="s">
+        <v>5</v>
+      </c>
+      <c r="P20" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3075,8 +3969,14 @@
       <c r="N21" t="s">
         <v>4</v>
       </c>
+      <c r="O21" t="s">
+        <v>4</v>
+      </c>
+      <c r="P21" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3116,8 +4016,14 @@
       <c r="N22" t="s">
         <v>4</v>
       </c>
+      <c r="O22" t="s">
+        <v>4</v>
+      </c>
+      <c r="P22" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -3157,8 +4063,14 @@
       <c r="N23" t="s">
         <v>4</v>
       </c>
+      <c r="O23" t="s">
+        <v>4</v>
+      </c>
+      <c r="P23" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -3198,8 +4110,14 @@
       <c r="N24" t="s">
         <v>4</v>
       </c>
+      <c r="O24" t="s">
+        <v>4</v>
+      </c>
+      <c r="P24" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -3236,8 +4154,14 @@
       <c r="N25" t="s">
         <v>4</v>
       </c>
+      <c r="O25" t="s">
+        <v>4</v>
+      </c>
+      <c r="P25" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -3277,8 +4201,14 @@
       <c r="N26" t="s">
         <v>4</v>
       </c>
+      <c r="O26" t="s">
+        <v>4</v>
+      </c>
+      <c r="P26" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -3318,8 +4248,14 @@
       <c r="N27" t="s">
         <v>4</v>
       </c>
+      <c r="O27" t="s">
+        <v>4</v>
+      </c>
+      <c r="P27" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -3359,8 +4295,14 @@
       <c r="N28" t="s">
         <v>5</v>
       </c>
+      <c r="O28" t="s">
+        <v>5</v>
+      </c>
+      <c r="P28" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -3400,8 +4342,14 @@
       <c r="N29" t="s">
         <v>4</v>
       </c>
+      <c r="O29" t="s">
+        <v>4</v>
+      </c>
+      <c r="P29" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -3441,8 +4389,14 @@
       <c r="N30" t="s">
         <v>4</v>
       </c>
+      <c r="O30" t="s">
+        <v>4</v>
+      </c>
+      <c r="P30" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -3482,8 +4436,14 @@
       <c r="N31" t="s">
         <v>4</v>
       </c>
+      <c r="O31" t="s">
+        <v>4</v>
+      </c>
+      <c r="P31" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -3523,8 +4483,14 @@
       <c r="N32" t="s">
         <v>4</v>
       </c>
+      <c r="O32" t="s">
+        <v>4</v>
+      </c>
+      <c r="P32" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -3564,8 +4530,14 @@
       <c r="N33" t="s">
         <v>4</v>
       </c>
+      <c r="O33" t="s">
+        <v>4</v>
+      </c>
+      <c r="P33" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -3605,8 +4577,14 @@
       <c r="N34" t="s">
         <v>4</v>
       </c>
+      <c r="O34" t="s">
+        <v>4</v>
+      </c>
+      <c r="P34" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -3646,8 +4624,14 @@
       <c r="N35" t="s">
         <v>4</v>
       </c>
+      <c r="O35" t="s">
+        <v>4</v>
+      </c>
+      <c r="P35" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -3687,8 +4671,14 @@
       <c r="N36" t="s">
         <v>4</v>
       </c>
+      <c r="O36" t="s">
+        <v>4</v>
+      </c>
+      <c r="P36" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -3728,8 +4718,14 @@
       <c r="N37" t="s">
         <v>4</v>
       </c>
+      <c r="O37" t="s">
+        <v>4</v>
+      </c>
+      <c r="P37" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -3769,8 +4765,14 @@
       <c r="N38" t="s">
         <v>5</v>
       </c>
+      <c r="O38" t="s">
+        <v>5</v>
+      </c>
+      <c r="P38" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -3810,8 +4812,14 @@
       <c r="N39" t="s">
         <v>4</v>
       </c>
+      <c r="O39" t="s">
+        <v>4</v>
+      </c>
+      <c r="P39" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -3851,8 +4859,14 @@
       <c r="N40" t="s">
         <v>4</v>
       </c>
+      <c r="O40" t="s">
+        <v>4</v>
+      </c>
+      <c r="P40" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -3892,8 +4906,14 @@
       <c r="N41" t="s">
         <v>4</v>
       </c>
+      <c r="O41" t="s">
+        <v>4</v>
+      </c>
+      <c r="P41" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -3933,8 +4953,14 @@
       <c r="N42" t="s">
         <v>4</v>
       </c>
+      <c r="O42" t="s">
+        <v>4</v>
+      </c>
+      <c r="P42" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -3971,8 +4997,14 @@
       <c r="N43" t="s">
         <v>4</v>
       </c>
+      <c r="O43" t="s">
+        <v>4</v>
+      </c>
+      <c r="P43" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -4009,8 +5041,14 @@
       <c r="N44" t="s">
         <v>4</v>
       </c>
+      <c r="O44" t="s">
+        <v>4</v>
+      </c>
+      <c r="P44" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -4047,8 +5085,14 @@
       <c r="N45" t="s">
         <v>4</v>
       </c>
+      <c r="O45" t="s">
+        <v>4</v>
+      </c>
+      <c r="P45" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -4085,8 +5129,14 @@
       <c r="N46" t="s">
         <v>4</v>
       </c>
+      <c r="O46" t="s">
+        <v>4</v>
+      </c>
+      <c r="P46" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -4123,8 +5173,14 @@
       <c r="N47" t="s">
         <v>4</v>
       </c>
+      <c r="O47" t="s">
+        <v>4</v>
+      </c>
+      <c r="P47" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -4161,8 +5217,14 @@
       <c r="N48" t="s">
         <v>4</v>
       </c>
+      <c r="O48" t="s">
+        <v>4</v>
+      </c>
+      <c r="P48" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -4199,8 +5261,14 @@
       <c r="N49" t="s">
         <v>4</v>
       </c>
+      <c r="O49" t="s">
+        <v>4</v>
+      </c>
+      <c r="P49" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -4237,8 +5305,14 @@
       <c r="N50" t="s">
         <v>4</v>
       </c>
+      <c r="O50" t="s">
+        <v>4</v>
+      </c>
+      <c r="P50" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -4275,512 +5349,870 @@
       <c r="N51" t="s">
         <v>4</v>
       </c>
+      <c r="O51" t="s">
+        <v>4</v>
+      </c>
+      <c r="P51" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D16 D52:D1048576">
-    <cfRule type="containsText" dxfId="226" priority="225" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="322" priority="321" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="227" priority="224" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="323" priority="320" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="225" priority="223" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="321" priority="319" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17:D19">
-    <cfRule type="containsText" dxfId="222" priority="220" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="318" priority="316" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="223" priority="221" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="319" priority="317" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="224" priority="222" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="320" priority="318" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",D17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="containsText" dxfId="219" priority="217" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="315" priority="313" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",D20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="220" priority="218" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="316" priority="314" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",D20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="221" priority="219" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="317" priority="315" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",D20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22">
-    <cfRule type="containsText" dxfId="213" priority="211" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="309" priority="307" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",D22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="214" priority="212" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="310" priority="308" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",D22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="215" priority="213" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="311" priority="309" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",D22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D24">
-    <cfRule type="containsText" dxfId="212" priority="208" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="308" priority="304" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="211" priority="209" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="307" priority="305" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="210" priority="210" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="306" priority="306" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="containsText" dxfId="204" priority="202" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="300" priority="298" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",D25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="205" priority="203" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="301" priority="299" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",D25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="206" priority="204" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="302" priority="300" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",D25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26:D28">
-    <cfRule type="containsText" dxfId="203" priority="199" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="299" priority="295" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",D26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="202" priority="200" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="298" priority="296" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",D26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="201" priority="201" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="297" priority="297" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",D26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29:D37">
-    <cfRule type="containsText" dxfId="200" priority="196" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="296" priority="292" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",D29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="199" priority="197" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="295" priority="293" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",D29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="198" priority="198" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="294" priority="294" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",D29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38:D39">
-    <cfRule type="containsText" dxfId="197" priority="193" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="293" priority="289" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",D38)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="196" priority="194" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="292" priority="290" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",D38)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="195" priority="195" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="291" priority="291" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",D38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43:D47">
-    <cfRule type="containsText" dxfId="189" priority="187" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="285" priority="283" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",D43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="190" priority="188" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="286" priority="284" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",D43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="191" priority="189" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="287" priority="285" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",D43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D49:D51">
-    <cfRule type="containsText" dxfId="188" priority="184" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="284" priority="280" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",D49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="187" priority="185" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="283" priority="281" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",D49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="186" priority="186" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="282" priority="282" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",D49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D48">
-    <cfRule type="containsText" dxfId="185" priority="181" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="281" priority="277" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",D48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="184" priority="182" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="280" priority="278" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",D48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="183" priority="183" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="279" priority="279" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",D48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I52:I1048576 I1:I16">
-    <cfRule type="containsText" dxfId="180" priority="178" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="276" priority="274" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="181" priority="179" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="277" priority="275" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="182" priority="180" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="278" priority="276" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17:I19">
-    <cfRule type="containsText" dxfId="179" priority="175" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="275" priority="271" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",I17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="178" priority="176" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="274" priority="272" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",I17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="177" priority="177" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="273" priority="273" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",I17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20">
-    <cfRule type="containsText" dxfId="176" priority="172" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="272" priority="268" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",I20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="175" priority="173" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="271" priority="269" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",I20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="174" priority="174" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="270" priority="270" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",I20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21">
-    <cfRule type="containsText" dxfId="173" priority="169" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="269" priority="265" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",I21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="172" priority="170" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="268" priority="266" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",I21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="171" priority="171" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="267" priority="267" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22">
-    <cfRule type="containsText" dxfId="170" priority="166" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="266" priority="262" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",I22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="169" priority="167" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="265" priority="263" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",I22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="168" priority="168" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="264" priority="264" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",I22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23">
-    <cfRule type="containsText" dxfId="167" priority="163" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="263" priority="259" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",I23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="166" priority="164" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="262" priority="260" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",I23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="165" priority="165" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="261" priority="261" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",I23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24">
-    <cfRule type="containsText" dxfId="164" priority="160" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="260" priority="256" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",I24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="163" priority="161" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="259" priority="257" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",I24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="162" priority="162" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="258" priority="258" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",I24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I25">
-    <cfRule type="containsText" dxfId="161" priority="157" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="257" priority="253" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",I25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="160" priority="158" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="256" priority="254" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",I25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="159" priority="159" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="255" priority="255" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",I25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26:I28">
-    <cfRule type="containsText" dxfId="158" priority="154" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="254" priority="250" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",I26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="157" priority="155" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="253" priority="251" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",I26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="156" priority="156" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="252" priority="252" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",I26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I29:I37">
-    <cfRule type="containsText" dxfId="155" priority="151" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="251" priority="247" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",I29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="154" priority="152" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="250" priority="248" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",I29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="153" priority="153" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="249" priority="249" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",I29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="containsText" dxfId="152" priority="148" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="248" priority="244" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",I38)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="151" priority="149" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="247" priority="245" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",I38)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="150" priority="150" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="246" priority="246" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",I38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39:I42">
-    <cfRule type="containsText" dxfId="149" priority="145" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="245" priority="241" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",I39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="148" priority="146" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="244" priority="242" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",I39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="147" priority="147" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="243" priority="243" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",I39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I43:I47">
-    <cfRule type="containsText" dxfId="146" priority="142" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="242" priority="238" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",I43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="145" priority="143" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="241" priority="239" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",I43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="144" priority="144" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="240" priority="240" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",I43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49:I51">
-    <cfRule type="containsText" dxfId="143" priority="139" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="239" priority="235" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",I49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="140" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="238" priority="236" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",I49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="141" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="237" priority="237" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",I49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I48">
-    <cfRule type="containsText" dxfId="140" priority="136" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="236" priority="232" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",I48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="139" priority="137" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="235" priority="233" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",I48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="138" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="234" priority="234" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",I48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N52:N1048576 N1">
-    <cfRule type="containsText" dxfId="137" priority="133" operator="containsText" text="wrong">
+    <cfRule type="containsText" dxfId="233" priority="229" operator="containsText" text="wrong">
       <formula>NOT(ISERROR(SEARCH("wrong",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="136" priority="134" operator="containsText" text="bad">
+    <cfRule type="containsText" dxfId="232" priority="230" operator="containsText" text="bad">
       <formula>NOT(ISERROR(SEARCH("bad",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="135" operator="containsText" text="good">
+    <cfRule type="containsText" dxfId="231" priority="231" operator="containsText" text="good">
       <formula>NOT(ISERROR(SEARCH("good",N1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21">
+    <cfRule type="containsText" dxfId="149" priority="148" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",D21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="148" priority="149" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",D21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="147" priority="150" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",D21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40:D41">
+    <cfRule type="containsText" dxfId="146" priority="145" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",D40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="145" priority="146" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",D40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="144" priority="147" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",D40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D42">
+    <cfRule type="containsText" dxfId="143" priority="142" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",D42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="142" priority="143" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",D42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="141" priority="144" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",D42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N16">
+    <cfRule type="containsText" dxfId="138" priority="139" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",N2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="139" priority="140" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",N2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="140" priority="141" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",N2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N17:N19">
+    <cfRule type="containsText" dxfId="137" priority="136" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",N17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="136" priority="137" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",N17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="135" priority="138" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",N17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N20">
+    <cfRule type="containsText" dxfId="134" priority="133" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",N20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="133" priority="134" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",N20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="132" priority="135" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",N20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N22">
+    <cfRule type="containsText" dxfId="131" priority="130" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",N22)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="130" priority="131" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",N22)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="129" priority="132" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",N22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N23:N24">
+    <cfRule type="containsText" dxfId="128" priority="127" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",N23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="127" priority="128" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",N23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="126" priority="129" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",N23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N25">
+    <cfRule type="containsText" dxfId="125" priority="124" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",N25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="124" priority="125" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",N25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="123" priority="126" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",N25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N26:N28">
+    <cfRule type="containsText" dxfId="122" priority="121" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",N26)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="121" priority="122" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",N26)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="120" priority="123" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",N26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N29:N37">
+    <cfRule type="containsText" dxfId="119" priority="118" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",N29)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="118" priority="119" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",N29)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="117" priority="120" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",N29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N38:N39">
+    <cfRule type="containsText" dxfId="116" priority="115" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",N38)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="115" priority="116" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",N38)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="114" priority="117" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",N38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N43:N47">
+    <cfRule type="containsText" dxfId="113" priority="112" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",N43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="112" priority="113" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",N43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="111" priority="114" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",N43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N49:N51">
+    <cfRule type="containsText" dxfId="110" priority="109" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",N49)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="109" priority="110" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",N49)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="108" priority="111" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",N49)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N48">
+    <cfRule type="containsText" dxfId="107" priority="106" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",N48)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="106" priority="107" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",N48)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="105" priority="108" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",N48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N21">
+    <cfRule type="containsText" dxfId="104" priority="103" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",N21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="103" priority="104" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",N21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="102" priority="105" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",N21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N40:N41">
+    <cfRule type="containsText" dxfId="101" priority="100" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",N40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="100" priority="101" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",N40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="99" priority="102" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",N40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N42">
+    <cfRule type="containsText" dxfId="98" priority="97" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",N42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="97" priority="98" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",N42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="96" priority="99" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",N42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O52:O1048576 O1">
+    <cfRule type="containsText" dxfId="95" priority="94" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",O1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="94" priority="95" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",O1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="93" priority="96" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",O1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:O16">
+    <cfRule type="containsText" dxfId="92" priority="91" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",O2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="91" priority="92" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",O2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="90" priority="93" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",O2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O17:O19">
+    <cfRule type="containsText" dxfId="89" priority="88" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",O17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="88" priority="89" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",O17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="87" priority="90" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",O17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O20">
+    <cfRule type="containsText" dxfId="86" priority="85" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",O20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="85" priority="86" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",O20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="84" priority="87" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",O20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O22">
+    <cfRule type="containsText" dxfId="83" priority="82" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",O22)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="82" priority="83" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",O22)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="81" priority="84" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",O22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O23:O24">
+    <cfRule type="containsText" dxfId="80" priority="79" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",O23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="79" priority="80" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",O23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="78" priority="81" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",O23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O25">
+    <cfRule type="containsText" dxfId="77" priority="76" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",O25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="76" priority="77" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",O25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="75" priority="78" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",O25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O26:O28">
+    <cfRule type="containsText" dxfId="74" priority="73" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",O26)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",O26)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="72" priority="75" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",O26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O29:O37">
+    <cfRule type="containsText" dxfId="71" priority="70" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",O29)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",O29)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="69" priority="72" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",O29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O38:O39">
+    <cfRule type="containsText" dxfId="68" priority="67" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",O38)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="67" priority="68" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",O38)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="66" priority="69" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",O38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O43:O47">
+    <cfRule type="containsText" dxfId="65" priority="64" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",O43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",O43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="63" priority="66" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",O43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O49:O51">
+    <cfRule type="containsText" dxfId="62" priority="61" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",O49)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",O49)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="60" priority="63" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",O49)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O48">
+    <cfRule type="containsText" dxfId="59" priority="58" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",O48)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",O48)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="57" priority="60" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",O48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O21">
+    <cfRule type="containsText" dxfId="56" priority="55" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",O21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="55" priority="56" operator="containsText" text="bad">
+      <formula>NOT(ISERROR(SEARCH("bad",O21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="54" priority="57" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",O21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O40:O41">
     <cfRule type="containsText" dxfId="53" priority="52" operator="containsText" text="wrong">
-      <formula>NOT(ISERROR(SEARCH("wrong",D21)))</formula>
+      <formula>NOT(ISERROR(SEARCH("wrong",O40)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="52" priority="53" operator="containsText" text="bad">
-      <formula>NOT(ISERROR(SEARCH("bad",D21)))</formula>
+      <formula>NOT(ISERROR(SEARCH("bad",O40)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="51" priority="54" operator="containsText" text="good">
-      <formula>NOT(ISERROR(SEARCH("good",D21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D40:D41">
+      <formula>NOT(ISERROR(SEARCH("good",O40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O42">
     <cfRule type="containsText" dxfId="50" priority="49" operator="containsText" text="wrong">
-      <formula>NOT(ISERROR(SEARCH("wrong",D40)))</formula>
+      <formula>NOT(ISERROR(SEARCH("wrong",O42)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="49" priority="50" operator="containsText" text="bad">
-      <formula>NOT(ISERROR(SEARCH("bad",D40)))</formula>
+      <formula>NOT(ISERROR(SEARCH("bad",O42)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="48" priority="51" operator="containsText" text="good">
-      <formula>NOT(ISERROR(SEARCH("good",D40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D42">
+      <formula>NOT(ISERROR(SEARCH("good",O42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P52:P1048576 P1">
     <cfRule type="containsText" dxfId="47" priority="46" operator="containsText" text="wrong">
-      <formula>NOT(ISERROR(SEARCH("wrong",D42)))</formula>
+      <formula>NOT(ISERROR(SEARCH("wrong",P1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="bad">
-      <formula>NOT(ISERROR(SEARCH("bad",D42)))</formula>
+      <formula>NOT(ISERROR(SEARCH("bad",P1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="45" priority="48" operator="containsText" text="good">
-      <formula>NOT(ISERROR(SEARCH("good",D42)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N16">
-    <cfRule type="containsText" dxfId="42" priority="43" operator="containsText" text="wrong">
-      <formula>NOT(ISERROR(SEARCH("wrong",N2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("good",P1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:P16">
+    <cfRule type="containsText" dxfId="44" priority="43" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH("wrong",P2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="43" priority="44" operator="containsText" text="bad">
-      <formula>NOT(ISERROR(SEARCH("bad",N2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="45" operator="containsText" text="good">
-      <formula>NOT(ISERROR(SEARCH("good",N2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N17:N19">
+      <formula>NOT(ISERROR(SEARCH("bad",P2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="45" operator="containsText" text="good">
+      <formula>NOT(ISERROR(SEARCH("good",P2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P17:P19">
     <cfRule type="containsText" dxfId="41" priority="40" operator="containsText" text="wrong">
-      <formula>NOT(ISERROR(SEARCH("wrong",N17)))</formula>
+      <formula>NOT(ISERROR(SEARCH("wrong",P17)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="bad">
-      <formula>NOT(ISERROR(SEARCH("bad",N17)))</formula>
+      <formula>NOT(ISERROR(SEARCH("bad",P17)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="39" priority="42" operator="containsText" text="good">
-      <formula>NOT(ISERROR(SEARCH("good",N17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N20">
+      <formula>NOT(ISERROR(SEARCH("good",P17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P20">
     <cfRule type="containsText" dxfId="38" priority="37" operator="containsText" text="wrong">
-      <formula>NOT(ISERROR(SEARCH("wrong",N20)))</formula>
+      <formula>NOT(ISERROR(SEARCH("wrong",P20)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="bad">
-      <formula>NOT(ISERROR(SEARCH("bad",N20)))</formula>
+      <formula>NOT(ISERROR(SEARCH("bad",P20)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="good">
-      <formula>NOT(ISERROR(SEARCH("good",N20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N22">
+      <formula>NOT(ISERROR(SEARCH("good",P20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P22">
     <cfRule type="containsText" dxfId="35" priority="34" operator="containsText" text="wrong">
-      <formula>NOT(ISERROR(SEARCH("wrong",N22)))</formula>
+      <formula>NOT(ISERROR(SEARCH("wrong",P22)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="bad">
-      <formula>NOT(ISERROR(SEARCH("bad",N22)))</formula>
+      <formula>NOT(ISERROR(SEARCH("bad",P22)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="good">
-      <formula>NOT(ISERROR(SEARCH("good",N22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N23:N24">
+      <formula>NOT(ISERROR(SEARCH("good",P22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P23:P24">
     <cfRule type="containsText" dxfId="32" priority="31" operator="containsText" text="wrong">
-      <formula>NOT(ISERROR(SEARCH("wrong",N23)))</formula>
+      <formula>NOT(ISERROR(SEARCH("wrong",P23)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="bad">
-      <formula>NOT(ISERROR(SEARCH("bad",N23)))</formula>
+      <formula>NOT(ISERROR(SEARCH("bad",P23)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="good">
-      <formula>NOT(ISERROR(SEARCH("good",N23)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N25">
+      <formula>NOT(ISERROR(SEARCH("good",P23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P25">
     <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="wrong">
-      <formula>NOT(ISERROR(SEARCH("wrong",N25)))</formula>
+      <formula>NOT(ISERROR(SEARCH("wrong",P25)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="bad">
-      <formula>NOT(ISERROR(SEARCH("bad",N25)))</formula>
+      <formula>NOT(ISERROR(SEARCH("bad",P25)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="good">
-      <formula>NOT(ISERROR(SEARCH("good",N25)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N26:N28">
+      <formula>NOT(ISERROR(SEARCH("good",P25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P26:P28">
     <cfRule type="containsText" dxfId="26" priority="25" operator="containsText" text="wrong">
-      <formula>NOT(ISERROR(SEARCH("wrong",N26)))</formula>
+      <formula>NOT(ISERROR(SEARCH("wrong",P26)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="bad">
-      <formula>NOT(ISERROR(SEARCH("bad",N26)))</formula>
+      <formula>NOT(ISERROR(SEARCH("bad",P26)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="good">
-      <formula>NOT(ISERROR(SEARCH("good",N26)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N29:N37">
+      <formula>NOT(ISERROR(SEARCH("good",P26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P29:P37">
     <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="wrong">
-      <formula>NOT(ISERROR(SEARCH("wrong",N29)))</formula>
+      <formula>NOT(ISERROR(SEARCH("wrong",P29)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="bad">
-      <formula>NOT(ISERROR(SEARCH("bad",N29)))</formula>
+      <formula>NOT(ISERROR(SEARCH("bad",P29)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="good">
-      <formula>NOT(ISERROR(SEARCH("good",N29)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N38:N39">
+      <formula>NOT(ISERROR(SEARCH("good",P29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P38:P39">
     <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="wrong">
-      <formula>NOT(ISERROR(SEARCH("wrong",N38)))</formula>
+      <formula>NOT(ISERROR(SEARCH("wrong",P38)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="bad">
-      <formula>NOT(ISERROR(SEARCH("bad",N38)))</formula>
+      <formula>NOT(ISERROR(SEARCH("bad",P38)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="good">
-      <formula>NOT(ISERROR(SEARCH("good",N38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N43:N47">
+      <formula>NOT(ISERROR(SEARCH("good",P38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P43:P47">
     <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="wrong">
-      <formula>NOT(ISERROR(SEARCH("wrong",N43)))</formula>
+      <formula>NOT(ISERROR(SEARCH("wrong",P43)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="bad">
-      <formula>NOT(ISERROR(SEARCH("bad",N43)))</formula>
+      <formula>NOT(ISERROR(SEARCH("bad",P43)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="good">
-      <formula>NOT(ISERROR(SEARCH("good",N43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N49:N51">
+      <formula>NOT(ISERROR(SEARCH("good",P43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P49:P51">
     <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="wrong">
-      <formula>NOT(ISERROR(SEARCH("wrong",N49)))</formula>
+      <formula>NOT(ISERROR(SEARCH("wrong",P49)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="bad">
-      <formula>NOT(ISERROR(SEARCH("bad",N49)))</formula>
+      <formula>NOT(ISERROR(SEARCH("bad",P49)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="good">
-      <formula>NOT(ISERROR(SEARCH("good",N49)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N48">
+      <formula>NOT(ISERROR(SEARCH("good",P49)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P48">
     <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="wrong">
-      <formula>NOT(ISERROR(SEARCH("wrong",N48)))</formula>
+      <formula>NOT(ISERROR(SEARCH("wrong",P48)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="bad">
-      <formula>NOT(ISERROR(SEARCH("bad",N48)))</formula>
+      <formula>NOT(ISERROR(SEARCH("bad",P48)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="good">
-      <formula>NOT(ISERROR(SEARCH("good",N48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N21">
+      <formula>NOT(ISERROR(SEARCH("good",P48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P21">
     <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="wrong">
-      <formula>NOT(ISERROR(SEARCH("wrong",N21)))</formula>
+      <formula>NOT(ISERROR(SEARCH("wrong",P21)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="bad">
-      <formula>NOT(ISERROR(SEARCH("bad",N21)))</formula>
+      <formula>NOT(ISERROR(SEARCH("bad",P21)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="good">
-      <formula>NOT(ISERROR(SEARCH("good",N21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N40:N41">
+      <formula>NOT(ISERROR(SEARCH("good",P21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P40:P41">
     <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="wrong">
-      <formula>NOT(ISERROR(SEARCH("wrong",N40)))</formula>
+      <formula>NOT(ISERROR(SEARCH("wrong",P40)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="bad">
-      <formula>NOT(ISERROR(SEARCH("bad",N40)))</formula>
+      <formula>NOT(ISERROR(SEARCH("bad",P40)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="good">
-      <formula>NOT(ISERROR(SEARCH("good",N40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N42">
+      <formula>NOT(ISERROR(SEARCH("good",P40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P42">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="wrong">
-      <formula>NOT(ISERROR(SEARCH("wrong",N42)))</formula>
+      <formula>NOT(ISERROR(SEARCH("wrong",P42)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="bad">
-      <formula>NOT(ISERROR(SEARCH("bad",N42)))</formula>
+      <formula>NOT(ISERROR(SEARCH("bad",P42)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="good">
-      <formula>NOT(ISERROR(SEARCH("good",N42)))</formula>
+      <formula>NOT(ISERROR(SEARCH("good",P42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>